<commit_message>
ajout xls, modification xlsx et ajout du pptx
</commit_message>
<xml_diff>
--- a/mon excell.xlsx
+++ b/mon excell.xlsx
@@ -63,6 +63,132 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="fr-FR"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$1:$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$1:$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="111543040"/>
+        <c:axId val="111544576"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="111543040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="111544576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="111544576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="111543040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -370,10 +496,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -394,8 +520,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>